<commit_message>
Top Offenders methods and levels plus libriries installer
</commit_message>
<xml_diff>
--- a/exported_dfs/107130-KNE United States_combined.xlsx
+++ b/exported_dfs/107130-KNE United States_combined.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ae3fc46a81f6f95/Desktop/Auto-Parameters-Tuning/exported_dfs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_C0F6812DF9789444283D346AA8FDF435905EFA00" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F26D07CE-70CA-432F-8463-8B9ABE8005D8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="11">
   <si>
     <t>Item</t>
   </si>
@@ -37,13 +31,7 @@
     <t>Act Orders Final Rev</t>
   </si>
   <si>
-    <t>Fcst Stat Prelim Rev_OutlierSensitivity_3</t>
-  </si>
-  <si>
-    <t>Fcst Stat Prelim Rev_OutliersPercent_5</t>
-  </si>
-  <si>
-    <t>Fcst Stat Prelim Rev_EnableNonNegRegr_1</t>
+    <t>Fcst Stat Prelim Rev_FitValidationSensitivity_1.7</t>
   </si>
   <si>
     <t>End of History</t>
@@ -64,11 +52,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,21 +120,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -184,7 +164,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -218,7 +198,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -253,10 +232,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -429,23 +407,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,22 +439,16 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
         <v>44501</v>
@@ -494,15 +457,15 @@
         <v>3948</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2">
         <v>44531</v>
@@ -511,24 +474,18 @@
         <v>5504</v>
       </c>
       <c r="F3">
-        <v>2417</v>
-      </c>
-      <c r="G3">
         <v>2308</v>
       </c>
-      <c r="H3">
-        <v>2308</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>44562</v>
@@ -537,24 +494,18 @@
         <v>3097</v>
       </c>
       <c r="F4">
-        <v>2519</v>
-      </c>
-      <c r="G4">
         <v>2308</v>
       </c>
-      <c r="H4">
-        <v>2308</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>44593</v>
@@ -563,24 +514,18 @@
         <v>3604</v>
       </c>
       <c r="F5">
-        <v>3018</v>
-      </c>
-      <c r="G5">
         <v>2665</v>
       </c>
-      <c r="H5">
-        <v>2665</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
         <v>44621</v>
@@ -589,24 +534,18 @@
         <v>4613</v>
       </c>
       <c r="F6">
-        <v>2905</v>
-      </c>
-      <c r="G6">
         <v>2665</v>
       </c>
-      <c r="H6">
-        <v>2665</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2">
         <v>44652</v>
@@ -615,24 +554,18 @@
         <v>3955</v>
       </c>
       <c r="F7">
-        <v>3382</v>
-      </c>
-      <c r="G7">
         <v>3020</v>
       </c>
-      <c r="H7">
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>44682</v>
@@ -641,24 +574,18 @@
         <v>3952</v>
       </c>
       <c r="F8">
-        <v>3258</v>
-      </c>
-      <c r="G8">
         <v>3020</v>
       </c>
-      <c r="H8">
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2">
         <v>44713</v>
@@ -667,24 +594,18 @@
         <v>4561</v>
       </c>
       <c r="F9">
-        <v>3622</v>
-      </c>
-      <c r="G9">
         <v>3373</v>
       </c>
-      <c r="H9">
-        <v>3373</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2">
         <v>44743</v>
@@ -693,24 +614,18 @@
         <v>4049</v>
       </c>
       <c r="F10">
-        <v>3550</v>
-      </c>
-      <c r="G10">
         <v>3373</v>
       </c>
-      <c r="H10">
-        <v>3373</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2">
         <v>44774</v>
@@ -719,24 +634,18 @@
         <v>4353</v>
       </c>
       <c r="F11">
-        <v>3902</v>
-      </c>
-      <c r="G11">
         <v>3724</v>
       </c>
-      <c r="H11">
-        <v>3724</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2">
         <v>44805</v>
@@ -745,24 +654,18 @@
         <v>4195</v>
       </c>
       <c r="F12">
-        <v>3837</v>
-      </c>
-      <c r="G12">
         <v>3724</v>
       </c>
-      <c r="H12">
-        <v>3724</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2">
         <v>44835</v>
@@ -771,24 +674,18 @@
         <v>4836</v>
       </c>
       <c r="F13">
-        <v>4190</v>
-      </c>
-      <c r="G13">
         <v>4074</v>
       </c>
-      <c r="H13">
-        <v>4074</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2">
         <v>44866</v>
@@ -797,24 +694,18 @@
         <v>5363</v>
       </c>
       <c r="F14">
-        <v>4166</v>
-      </c>
-      <c r="G14">
         <v>4074</v>
       </c>
-      <c r="H14">
-        <v>4074</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2">
         <v>44896</v>
@@ -823,24 +714,18 @@
         <v>7184</v>
       </c>
       <c r="F15">
-        <v>4188</v>
-      </c>
-      <c r="G15">
         <v>4074</v>
       </c>
-      <c r="H15">
-        <v>4074</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2">
         <v>44927</v>
@@ -849,24 +734,18 @@
         <v>4357</v>
       </c>
       <c r="F16">
-        <v>4724</v>
-      </c>
-      <c r="G16">
         <v>4421</v>
       </c>
-      <c r="H16">
-        <v>4421</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2">
         <v>44958</v>
@@ -875,24 +754,18 @@
         <v>3805</v>
       </c>
       <c r="F17">
-        <v>4608</v>
-      </c>
-      <c r="G17">
         <v>4421</v>
       </c>
-      <c r="H17">
-        <v>4421</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2">
         <v>44986</v>
@@ -901,24 +774,18 @@
         <v>5134</v>
       </c>
       <c r="F18">
-        <v>4478</v>
-      </c>
-      <c r="G18">
         <v>4421</v>
       </c>
-      <c r="H18">
-        <v>4421</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
         <v>45017</v>
@@ -927,24 +794,18 @@
         <v>4187</v>
       </c>
       <c r="F19">
-        <v>4844</v>
-      </c>
-      <c r="G19">
         <v>4766</v>
       </c>
-      <c r="H19">
-        <v>4766</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2">
         <v>45047</v>
@@ -953,24 +814,18 @@
         <v>5070</v>
       </c>
       <c r="F20">
-        <v>4765</v>
-      </c>
-      <c r="G20">
         <v>4766</v>
       </c>
-      <c r="H20">
-        <v>4766</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2">
         <v>45078</v>
@@ -981,22 +836,16 @@
       <c r="F21">
         <v>4766</v>
       </c>
-      <c r="G21">
-        <v>4766</v>
-      </c>
-      <c r="H21">
-        <v>4766</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2">
         <v>45108</v>
@@ -1005,24 +854,18 @@
         <v>4058</v>
       </c>
       <c r="F22">
-        <v>5174</v>
-      </c>
-      <c r="G22">
         <v>5110</v>
       </c>
-      <c r="H22">
-        <v>5110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D23" s="2">
         <v>45139</v>
@@ -1031,24 +874,18 @@
         <v>5142</v>
       </c>
       <c r="F23">
-        <v>5090</v>
-      </c>
-      <c r="G23">
         <v>5110</v>
       </c>
-      <c r="H23">
-        <v>5110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D24" s="2">
         <v>45170</v>
@@ -1057,24 +894,18 @@
         <v>4674</v>
       </c>
       <c r="F24">
-        <v>5089</v>
-      </c>
-      <c r="G24">
         <v>5110</v>
       </c>
-      <c r="H24">
-        <v>5110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D25" s="2">
         <v>45200</v>
@@ -1083,24 +914,18 @@
         <v>5635</v>
       </c>
       <c r="F25">
-        <v>5428</v>
-      </c>
-      <c r="G25">
         <v>5452</v>
       </c>
-      <c r="H25">
-        <v>5452</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D26" s="2">
         <v>45231</v>
@@ -1109,24 +934,18 @@
         <v>5708</v>
       </c>
       <c r="F26">
-        <v>5444</v>
-      </c>
-      <c r="G26">
         <v>5452</v>
       </c>
-      <c r="H26">
-        <v>5452</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D27" s="2">
         <v>45261</v>
@@ -1135,24 +954,18 @@
         <v>8414</v>
       </c>
       <c r="F27">
-        <v>5463</v>
-      </c>
-      <c r="G27">
         <v>5452</v>
       </c>
-      <c r="H27">
-        <v>5452</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D28" s="2">
         <v>45292</v>
@@ -1161,24 +974,18 @@
         <v>4418</v>
       </c>
       <c r="F28">
-        <v>5629</v>
-      </c>
-      <c r="G28">
         <v>5452</v>
       </c>
-      <c r="H28">
-        <v>5452</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D29" s="2">
         <v>45323</v>
@@ -1187,24 +994,18 @@
         <v>5152</v>
       </c>
       <c r="F29">
-        <v>5885</v>
-      </c>
-      <c r="G29">
         <v>5791</v>
       </c>
-      <c r="H29">
-        <v>5791</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D30" s="2">
         <v>45352</v>
@@ -1213,24 +1014,18 @@
         <v>5065</v>
       </c>
       <c r="F30">
-        <v>5797</v>
-      </c>
-      <c r="G30">
         <v>5791</v>
       </c>
-      <c r="H30">
-        <v>5791</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D31" s="2">
         <v>45383</v>
@@ -1239,24 +1034,18 @@
         <v>5902</v>
       </c>
       <c r="F31">
-        <v>5736</v>
-      </c>
-      <c r="G31">
         <v>5791</v>
       </c>
-      <c r="H31">
-        <v>5791</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D32" s="2">
         <v>45413</v>
@@ -1265,24 +1054,18 @@
         <v>5772</v>
       </c>
       <c r="F32">
-        <v>5751</v>
-      </c>
-      <c r="G32">
         <v>5791</v>
       </c>
-      <c r="H32">
-        <v>5791</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D33" s="2">
         <v>45444</v>
@@ -1291,24 +1074,18 @@
         <v>5380</v>
       </c>
       <c r="F33">
-        <v>6119</v>
-      </c>
-      <c r="G33">
         <v>6129</v>
       </c>
-      <c r="H33">
-        <v>6129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D34" s="2">
         <v>45474</v>
@@ -1317,27 +1094,21 @@
         <v>5134</v>
       </c>
       <c r="F34">
-        <v>6083</v>
-      </c>
-      <c r="G34">
         <v>6129</v>
       </c>
       <c r="H34">
-        <v>6129</v>
-      </c>
-      <c r="J34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D35" s="2">
         <v>45505</v>
@@ -1346,24 +1117,18 @@
         <v>5376</v>
       </c>
       <c r="F35">
-        <v>6042</v>
-      </c>
-      <c r="G35">
         <v>6129</v>
       </c>
-      <c r="H35">
-        <v>6129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D36" s="2">
         <v>45536</v>
@@ -1372,27 +1137,21 @@
         <v>5869</v>
       </c>
       <c r="F36">
-        <v>6030</v>
-      </c>
-      <c r="G36">
         <v>6129</v>
       </c>
       <c r="H36">
-        <v>6129</v>
-      </c>
-      <c r="J36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D37" s="2">
         <v>45566</v>
@@ -1401,24 +1160,18 @@
         <v>6552</v>
       </c>
       <c r="F37">
-        <v>6402</v>
-      </c>
-      <c r="G37">
         <v>6465</v>
       </c>
-      <c r="H37">
-        <v>6465</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D38" s="2">
         <v>45597</v>
@@ -1427,889 +1180,655 @@
         <v>3412</v>
       </c>
       <c r="F38">
-        <v>6438</v>
+        <v>6465</v>
       </c>
       <c r="G38">
-        <v>6465</v>
-      </c>
-      <c r="H38">
-        <v>6465</v>
-      </c>
-      <c r="I38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D39" s="2">
         <v>45627</v>
       </c>
       <c r="F39">
-        <v>6438</v>
-      </c>
-      <c r="G39">
         <v>6465</v>
       </c>
-      <c r="H39">
-        <v>6465</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D40" s="2">
         <v>45658</v>
       </c>
       <c r="F40">
-        <v>6445</v>
-      </c>
-      <c r="G40">
         <v>6465</v>
       </c>
-      <c r="H40">
-        <v>6465</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D41" s="2">
         <v>45689</v>
       </c>
       <c r="F41">
-        <v>6449</v>
-      </c>
-      <c r="G41">
         <v>6465</v>
       </c>
-      <c r="H41">
-        <v>6465</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D42" s="2">
         <v>45717</v>
       </c>
       <c r="F42">
-        <v>6450</v>
-      </c>
-      <c r="G42">
         <v>6465</v>
       </c>
-      <c r="H42">
-        <v>6465</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D43" s="2">
         <v>45748</v>
       </c>
       <c r="F43">
-        <v>6800</v>
-      </c>
-      <c r="G43">
         <v>6799</v>
       </c>
-      <c r="H43">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D44" s="2">
         <v>45778</v>
       </c>
       <c r="F44">
-        <v>6801</v>
-      </c>
-      <c r="G44">
         <v>6799</v>
       </c>
-      <c r="H44">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D45" s="2">
         <v>45809</v>
       </c>
       <c r="F45">
-        <v>6801</v>
-      </c>
-      <c r="G45">
         <v>6799</v>
       </c>
-      <c r="H45">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D46" s="2">
         <v>45839</v>
       </c>
       <c r="F46">
-        <v>6801</v>
-      </c>
-      <c r="G46">
         <v>6799</v>
       </c>
-      <c r="H46">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D47" s="2">
         <v>45870</v>
       </c>
       <c r="F47">
-        <v>6801</v>
-      </c>
-      <c r="G47">
         <v>6799</v>
       </c>
-      <c r="H47">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D48" s="2">
         <v>45901</v>
       </c>
       <c r="F48">
-        <v>6801</v>
-      </c>
-      <c r="G48">
         <v>6799</v>
       </c>
-      <c r="H48">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D49" s="2">
         <v>45931</v>
       </c>
       <c r="F49">
-        <v>6801</v>
-      </c>
-      <c r="G49">
         <v>6799</v>
       </c>
-      <c r="H49">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D50" s="2">
         <v>45962</v>
       </c>
       <c r="F50">
-        <v>6801</v>
-      </c>
-      <c r="G50">
         <v>6799</v>
       </c>
-      <c r="H50">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D51" s="2">
         <v>45992</v>
       </c>
       <c r="F51">
-        <v>6801</v>
-      </c>
-      <c r="G51">
         <v>6799</v>
       </c>
-      <c r="H51">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D52" s="2">
         <v>46023</v>
       </c>
       <c r="F52">
-        <v>6801</v>
-      </c>
-      <c r="G52">
         <v>6799</v>
       </c>
-      <c r="H52">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D53" s="2">
         <v>46054</v>
       </c>
       <c r="F53">
-        <v>6801</v>
-      </c>
-      <c r="G53">
         <v>6799</v>
       </c>
-      <c r="H53">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D54" s="2">
         <v>46082</v>
       </c>
       <c r="F54">
-        <v>6801</v>
-      </c>
-      <c r="G54">
         <v>6799</v>
       </c>
-      <c r="H54">
-        <v>6799</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D55" s="2">
         <v>46113</v>
       </c>
       <c r="F55">
-        <v>7149</v>
-      </c>
-      <c r="G55">
         <v>7131</v>
       </c>
-      <c r="H55">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D56" s="2">
         <v>46143</v>
       </c>
       <c r="F56">
-        <v>7149</v>
-      </c>
-      <c r="G56">
         <v>7131</v>
       </c>
-      <c r="H56">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D57" s="2">
         <v>46174</v>
       </c>
       <c r="F57">
-        <v>7149</v>
-      </c>
-      <c r="G57">
         <v>7131</v>
       </c>
-      <c r="H57">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D58" s="2">
         <v>46204</v>
       </c>
       <c r="F58">
-        <v>7149</v>
-      </c>
-      <c r="G58">
         <v>7131</v>
       </c>
-      <c r="H58">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D59" s="2">
         <v>46235</v>
       </c>
       <c r="F59">
-        <v>7149</v>
-      </c>
-      <c r="G59">
         <v>7131</v>
       </c>
-      <c r="H59">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D60" s="2">
         <v>46266</v>
       </c>
       <c r="F60">
-        <v>7149</v>
-      </c>
-      <c r="G60">
         <v>7131</v>
       </c>
-      <c r="H60">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D61" s="2">
         <v>46296</v>
       </c>
       <c r="F61">
-        <v>7149</v>
-      </c>
-      <c r="G61">
         <v>7131</v>
       </c>
-      <c r="H61">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D62" s="2">
         <v>46327</v>
       </c>
       <c r="F62">
-        <v>7149</v>
-      </c>
-      <c r="G62">
         <v>7131</v>
       </c>
-      <c r="H62">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D63" s="2">
         <v>46357</v>
       </c>
       <c r="F63">
-        <v>7149</v>
-      </c>
-      <c r="G63">
         <v>7131</v>
       </c>
-      <c r="H63">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D64" s="2">
         <v>46388</v>
       </c>
       <c r="F64">
-        <v>7149</v>
-      </c>
-      <c r="G64">
         <v>7131</v>
       </c>
-      <c r="H64">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D65" s="2">
         <v>46419</v>
       </c>
       <c r="F65">
-        <v>7149</v>
-      </c>
-      <c r="G65">
         <v>7131</v>
       </c>
-      <c r="H65">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D66" s="2">
         <v>46447</v>
       </c>
       <c r="F66">
-        <v>7149</v>
-      </c>
-      <c r="G66">
         <v>7131</v>
       </c>
-      <c r="H66">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D67" s="2">
         <v>46478</v>
       </c>
       <c r="F67">
-        <v>7149</v>
-      </c>
-      <c r="G67">
         <v>7131</v>
       </c>
-      <c r="H67">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D68" s="2">
         <v>46508</v>
       </c>
       <c r="F68">
-        <v>7149</v>
-      </c>
-      <c r="G68">
         <v>7131</v>
       </c>
-      <c r="H68">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D69" s="2">
         <v>46539</v>
       </c>
       <c r="F69">
-        <v>7495</v>
-      </c>
-      <c r="G69">
         <v>7462</v>
       </c>
-      <c r="H69">
-        <v>7462</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D70" s="2">
         <v>46569</v>
       </c>
       <c r="F70">
-        <v>7495</v>
-      </c>
-      <c r="G70">
         <v>7462</v>
       </c>
-      <c r="H70">
-        <v>7462</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D71" s="2">
         <v>46600</v>
       </c>
       <c r="F71">
-        <v>7495</v>
-      </c>
-      <c r="G71">
         <v>7462</v>
       </c>
-      <c r="H71">
-        <v>7462</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D72" s="2">
         <v>46631</v>
       </c>
       <c r="F72">
-        <v>7495</v>
-      </c>
-      <c r="G72">
         <v>7462</v>
       </c>
-      <c r="H72">
-        <v>7462</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D73" s="2">
         <v>46661</v>
       </c>
       <c r="F73">
-        <v>7495</v>
-      </c>
-      <c r="G73">
         <v>7462</v>
       </c>
-      <c r="H73">
-        <v>7462</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D74" s="2">
         <v>46692</v>
       </c>
       <c r="F74">
-        <v>7495</v>
-      </c>
-      <c r="G74">
         <v>7462</v>
       </c>
-      <c r="H74">
-        <v>7462</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D75" s="2">
         <v>46722</v>
       </c>
       <c r="F75">
-        <v>1389</v>
-      </c>
-      <c r="G75">
         <v>1588</v>
       </c>
-      <c r="H75">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D76" s="2">
         <v>46753</v>
       </c>
       <c r="F76">
-        <v>1389</v>
-      </c>
-      <c r="G76">
-        <v>1588</v>
-      </c>
-      <c r="H76">
         <v>1588</v>
       </c>
     </row>

</xml_diff>